<commit_message>
added gerbers for regulator board
</commit_message>
<xml_diff>
--- a/Speaker Boxes/Crossover/Crossover Measurements.xlsx
+++ b/Speaker Boxes/Crossover/Crossover Measurements.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="840" windowWidth="38400" windowHeight="21160" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12800" windowHeight="15480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -714,11 +714,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2081540008"/>
-        <c:axId val="2081537016"/>
+        <c:axId val="2072114328"/>
+        <c:axId val="2072111400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2081540008"/>
+        <c:axId val="2072114328"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -730,12 +730,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2081537016"/>
+        <c:crossAx val="2072111400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2081537016"/>
+        <c:axId val="2072111400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -747,7 +747,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2081540008"/>
+        <c:crossAx val="2072114328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1359,11 +1359,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2082241272"/>
-        <c:axId val="2082181048"/>
+        <c:axId val="2071305688"/>
+        <c:axId val="2071302696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2082241272"/>
+        <c:axId val="2071305688"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1375,12 +1375,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2082181048"/>
+        <c:crossAx val="2071302696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2082181048"/>
+        <c:axId val="2071302696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1392,7 +1392,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2082241272"/>
+        <c:crossAx val="2071305688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1448,16 +1448,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>81</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1803,7 +1803,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C40" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
       <selection activeCell="B150" sqref="B150"/>
     </sheetView>
   </sheetViews>
@@ -4421,7 +4421,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>